<commit_message>
Updated readme.md file and removed sleep
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HDFC_Automation\EntrataTest_SDET\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\EntrataTest_SDET\EntrataTest_SDET\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FE97B5-5814-40E2-8B4B-49ED13F6EAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="4575"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="1" r:id="rId1"/>
@@ -123,7 +124,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -208,15 +209,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -225,7 +225,7 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -510,81 +510,81 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="40.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="6" collapsed="1"/>
+    <col min="2" max="2" width="40.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.109375" style="5" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C8"/>
     </row>
   </sheetData>
@@ -594,148 +594,148 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C2" t="s">
@@ -750,7 +750,7 @@
       <c r="F2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H2">
@@ -759,45 +759,45 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="G2" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>